<commit_message>
added DFWT_TC_14 to DFWT_TC_20
</commit_message>
<xml_diff>
--- a/DFWT Change Request Update.xlsx
+++ b/DFWT Change Request Update.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="103">
   <si>
     <t>Change Request #</t>
   </si>
@@ -273,7 +273,132 @@
     <t>Verify if a user clicks “Add to Group” then it should move a specific Die Revision/Bank to the selected Group.</t>
   </si>
   <si>
-    <t>DFWT_CR_14</t>
+    <t>Verify upon creating a new project, success notification dialog will appear with info "Project &lt;project name&gt; has been successfully added."</t>
+  </si>
+  <si>
+    <t>After creating a Team Members, a dialog will popup that says "&lt;Name&gt;  was successfully added as a project member."</t>
+  </si>
+  <si>
+    <t>DFWT_TC_14</t>
+  </si>
+  <si>
+    <t>DFWT_TC_15</t>
+  </si>
+  <si>
+    <t>DFWT_TC_16</t>
+  </si>
+  <si>
+    <t>DFWT_TC_17</t>
+  </si>
+  <si>
+    <t>DFWT_TC_18</t>
+  </si>
+  <si>
+    <t>Verify after clicking Add Team Members, a dialog will pop up that contains input field of [Employee ID, Full Name, Functions].</t>
+  </si>
+  <si>
+    <t>Verify if clicking Add Contributor button,  a dialog will pop up that contains input field of [Function, Employee ID, Full Name].</t>
+  </si>
+  <si>
+    <t>Verify if adding one or more persons with the same function, a dialog will pop up with "&lt;name&gt; was successfully added as contributor." and Type column will set to "CONTRIBUTOR".</t>
+  </si>
+  <si>
+    <t>Verify if clicking Add Group Follower, "ADD SIGNOFF GROUP" dialog will pop up.</t>
+  </si>
+  <si>
+    <t>Verify if Team Member function can only exist once per project. If a user adds a new team member where a function was already assigned to someone, an alert dialog will pop up that says "&lt;functionName&gt; function is already assigned to a user. Please enter a new user or new function."</t>
+  </si>
+  <si>
+    <t>Verify upon creating a pool, a notification will pop up if the Pool name already exist. Otherwise a successful notification will pop up.</t>
+  </si>
+  <si>
+    <t>Verify if clicking Add ID Poll button, and adding a device ID using excel file, it will populate all devices from excel file.</t>
+  </si>
+  <si>
+    <t>Verify when adding a new Device ID using a pencil icon, which is already existed in a newly created Pool, a warning will show "This Device Id's Already Exist: "</t>
+  </si>
+  <si>
+    <t>Verify when clicking the trash bin icon to delete a Device ID in the pool, a notification dialog will show for confirmation.</t>
+  </si>
+  <si>
+    <t>Verify if the status of the Device ID is "RESERVED", it can't be deleted.</t>
+  </si>
+  <si>
+    <t>Verify if clicking the Device ID Mapping button, a notification will pop up if the project has no pool yet.</t>
+  </si>
+  <si>
+    <t>Verify when selecting a device ID's to reserve for a project, any checkboxes could only be check if "Number of ID selected" is less than the "Number of ID to reserve".</t>
+  </si>
+  <si>
+    <t>Verify when clicking Auto select Id button, checkboxes that are checked should be equal to the number of "Number of ID to reserve".</t>
+  </si>
+  <si>
+    <t>Verify when clicking Add New Product button, a dialog will pop up.</t>
+  </si>
+  <si>
+    <t>DFWT_TC_19</t>
+  </si>
+  <si>
+    <t>Verify when clicking trash bin icon to delete a Product, a delete confirmation dialog will pop up.</t>
+  </si>
+  <si>
+    <t>Verify upon delete a Product, a dialog will pop up saying "Product &lt;productName&gt; (MASTER) has been successfully deleted."</t>
+  </si>
+  <si>
+    <t>Verify upon creating a new Product, a dialog will pop up saying "Product &lt;productName&gt; has been successfully added."</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify when clicking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> icon to Add New Package Parent, a dialog box will show.</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify upon clicking Add button,  new package parent will be added in the product and package parent table.</t>
+  </si>
+  <si>
+    <t>Verify when clicking trash bin to Delete Package Parent, a delete confirmation dialog will pop up.</t>
+  </si>
+  <si>
+    <t>Verify upon clicking Yes button to delete package parent,  The package parent you removed will be deleted in the product and package parent table.</t>
+  </si>
+  <si>
+    <t>Verify when clicking the pencil icon besides the product, a dialog will pop up for renaming a product.</t>
+  </si>
+  <si>
+    <t>Verify upon clicking the Confirm button to rename a product, the new name of the product will be updated on the table.</t>
+  </si>
+  <si>
+    <t>Verify when clicking the pencil icon besides the package parent a dialog will pop up for renaming a  package parent</t>
+  </si>
+  <si>
+    <t>Verify upon clicking the Confirm button to rename a  package parent, the new name of the  package parent will be updated on the table.</t>
+  </si>
+  <si>
+    <t>Verify when clicking Comment button to edit die revision comment, a dialog will pop up to for editing a die revison comment.</t>
+  </si>
+  <si>
+    <t>DFWT_TC_20</t>
   </si>
 </sst>
 </file>
@@ -304,7 +429,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,8 +472,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -408,11 +539,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -468,6 +617,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -788,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1195,32 +1374,1185 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
+      <c r="C15" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="26"/>
+      <c r="B17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="1:11" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="28"/>
+      <c r="B20" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="25"/>
+      <c r="B23" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="25"/>
+      <c r="B24" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="25"/>
+      <c r="B25" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="25"/>
+      <c r="B26" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="25"/>
+      <c r="B27" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="25"/>
+      <c r="B28" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="25"/>
+      <c r="B29" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="25"/>
+      <c r="B31" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="25"/>
+      <c r="B32" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="25"/>
+      <c r="B33" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+    </row>
+    <row r="34" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34" s="25"/>
+      <c r="B34" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+    </row>
+    <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="25"/>
+      <c r="B35" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="25"/>
+      <c r="B36" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+    </row>
+    <row r="37" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="25"/>
+      <c r="B37" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+    </row>
+    <row r="38" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="25"/>
+      <c r="B38" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+    </row>
+    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A39" s="25"/>
+      <c r="B39" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+    </row>
+    <row r="40" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="25"/>
+      <c r="B40" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+    </row>
+    <row r="41" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="25"/>
+      <c r="B41" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="25"/>
+      <c r="B42" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="22">
+        <v>43966</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="22">
+        <v>43966</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A43" s="25"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A44" s="25"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A45" s="25"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A46" s="25"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A47" s="24"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A48" s="24"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A49" s="24"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A50" s="24"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A51" s="24"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A52" s="24"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A53" s="24"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A54" s="24"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A55" s="24"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A56" s="24"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A57" s="24"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A58" s="24"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="7"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A59" s="24"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A60" s="24"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A61" s="24"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A62" s="24"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="7"/>
+      <c r="K62" s="7"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A63" s="24"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A64" s="24"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A65" s="24"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A66" s="24"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+      <c r="I66" s="7"/>
+      <c r="J66" s="7"/>
+      <c r="K66" s="7"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A67" s="24"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A68" s="24"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A69" s="24"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A70" s="24"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="7"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A71" s="24"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A72" s="24"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="7"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="7"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A73" s="24"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="7"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A74" s="24"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+      <c r="I74" s="7"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="7"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A75" s="24"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+      <c r="K75" s="7"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A76" s="24"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="7"/>
+      <c r="J76" s="7"/>
+      <c r="K76" s="7"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A77" s="24"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="7"/>
+      <c r="J77" s="7"/>
+      <c r="K77" s="7"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A78" s="23"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="I78" s="7"/>
+      <c r="J78" s="7"/>
+      <c r="K78" s="7"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A79" s="23"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+      <c r="I79" s="7"/>
+      <c r="J79" s="7"/>
+      <c r="K79" s="7"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A80" s="20"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+      <c r="I80" s="7"/>
+      <c r="J80" s="7"/>
+      <c r="K80" s="7"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="11" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="12" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" s="12" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A30:A46"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A22:A29"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -1265,10 +2597,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="30">
         <v>3</v>
       </c>
       <c r="C2" s="6"/>
@@ -1281,8 +2613,8 @@
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="s">
         <v>41</v>
@@ -1293,8 +2625,8 @@
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7" t="s">
         <v>42</v>
@@ -1328,108 +2660,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="25" t="s">
+      <c r="C1" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="24" t="s">
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24" t="s">
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="25" t="s">
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
+      <c r="Y3" s="35"/>
+      <c r="Z3" s="35"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="13" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
added DFWT-WIPRO katalon project
</commit_message>
<xml_diff>
--- a/DFWT Change Request Update.xlsx
+++ b/DFWT Change Request Update.xlsx
@@ -778,6 +778,18 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -787,12 +799,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -810,12 +816,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1120,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1551,7 +1551,7 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="32" t="s">
         <v>71</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -1576,7 +1576,7 @@
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="28"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="7" t="s">
         <v>69</v>
       </c>
@@ -1591,7 +1591,7 @@
       <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="28"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="2" t="s">
         <v>127</v>
       </c>
@@ -1639,7 +1639,7 @@
       <c r="K19" s="7"/>
     </row>
     <row r="20" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="33" t="s">
         <v>73</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1664,7 +1664,7 @@
       <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="30"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="7" t="s">
         <v>77</v>
       </c>
@@ -1712,7 +1712,7 @@
       <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="29" t="s">
         <v>89</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -1737,7 +1737,7 @@
       <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="32"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="7" t="s">
         <v>80</v>
       </c>
@@ -1760,7 +1760,7 @@
       <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="32"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="7" t="s">
         <v>82</v>
       </c>
@@ -1783,7 +1783,7 @@
       <c r="K25" s="7"/>
     </row>
     <row r="26" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="32"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="7" t="s">
         <v>83</v>
       </c>
@@ -1806,7 +1806,7 @@
       <c r="K26" s="7"/>
     </row>
     <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="32"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="7" t="s">
         <v>84</v>
       </c>
@@ -1829,7 +1829,7 @@
       <c r="K27" s="7"/>
     </row>
     <row r="28" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="32"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="7" t="s">
         <v>85</v>
       </c>
@@ -1852,7 +1852,7 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="32"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="7" t="s">
         <v>86</v>
       </c>
@@ -1875,7 +1875,7 @@
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="32"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="7" t="s">
         <v>87</v>
       </c>
@@ -1898,7 +1898,7 @@
       <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="29" t="s">
         <v>102</v>
       </c>
       <c r="B31" s="7" t="s">
@@ -1923,7 +1923,7 @@
       <c r="K31" s="7"/>
     </row>
     <row r="32" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="32"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="7" t="s">
         <v>92</v>
       </c>
@@ -1946,7 +1946,7 @@
       <c r="K32" s="7"/>
     </row>
     <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="32"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="7" t="s">
         <v>90</v>
       </c>
@@ -1969,7 +1969,7 @@
       <c r="K33" s="7"/>
     </row>
     <row r="34" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="32"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="7" t="s">
         <v>91</v>
       </c>
@@ -1992,7 +1992,7 @@
       <c r="K34" s="7"/>
     </row>
     <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="32"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="7" t="s">
         <v>93</v>
       </c>
@@ -2015,7 +2015,7 @@
       <c r="K35" s="7"/>
     </row>
     <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="32"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="7" t="s">
         <v>94</v>
       </c>
@@ -2038,7 +2038,7 @@
       <c r="K36" s="7"/>
     </row>
     <row r="37" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="32"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="7" t="s">
         <v>95</v>
       </c>
@@ -2061,7 +2061,7 @@
       <c r="K37" s="7"/>
     </row>
     <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="32"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="7" t="s">
         <v>96</v>
       </c>
@@ -2084,7 +2084,7 @@
       <c r="K38" s="7"/>
     </row>
     <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="32"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="7" t="s">
         <v>97</v>
       </c>
@@ -2107,7 +2107,7 @@
       <c r="K39" s="7"/>
     </row>
     <row r="40" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="32"/>
+      <c r="A40" s="30"/>
       <c r="B40" s="7" t="s">
         <v>98</v>
       </c>
@@ -2130,7 +2130,7 @@
       <c r="K40" s="7"/>
     </row>
     <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="32"/>
+      <c r="A41" s="30"/>
       <c r="B41" s="7" t="s">
         <v>99</v>
       </c>
@@ -2153,7 +2153,7 @@
       <c r="K41" s="7"/>
     </row>
     <row r="42" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="32"/>
+      <c r="A42" s="30"/>
       <c r="B42" s="7" t="s">
         <v>100</v>
       </c>
@@ -2176,7 +2176,7 @@
       <c r="K42" s="7"/>
     </row>
     <row r="43" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="32"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="7" t="s">
         <v>101</v>
       </c>
@@ -2199,7 +2199,7 @@
       <c r="K43" s="7"/>
     </row>
     <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="32"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="7" t="s">
         <v>103</v>
       </c>
@@ -2222,7 +2222,7 @@
       <c r="K44" s="7"/>
     </row>
     <row r="45" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="32"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="7" t="s">
         <v>104</v>
       </c>
@@ -2245,7 +2245,7 @@
       <c r="K45" s="7"/>
     </row>
     <row r="46" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="32"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="7" t="s">
         <v>122</v>
       </c>
@@ -2268,7 +2268,7 @@
       <c r="K46" s="7"/>
     </row>
     <row r="47" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A47" s="32"/>
+      <c r="A47" s="30"/>
       <c r="B47" s="7" t="s">
         <v>121</v>
       </c>
@@ -2291,7 +2291,7 @@
       <c r="K47" s="7"/>
     </row>
     <row r="48" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="32"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="7" t="s">
         <v>120</v>
       </c>
@@ -2314,7 +2314,7 @@
       <c r="K48" s="7"/>
     </row>
     <row r="49" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="32"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="7" t="s">
         <v>123</v>
       </c>
@@ -2337,7 +2337,7 @@
       <c r="K49" s="7"/>
     </row>
     <row r="50" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="32"/>
+      <c r="A50" s="30"/>
       <c r="B50" s="7" t="s">
         <v>124</v>
       </c>
@@ -2360,7 +2360,7 @@
       <c r="K50" s="7"/>
     </row>
     <row r="51" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="39"/>
+      <c r="A51" s="31"/>
       <c r="B51" s="7" t="s">
         <v>125</v>
       </c>
@@ -2383,7 +2383,7 @@
       <c r="K51" s="7"/>
     </row>
     <row r="52" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="29" t="s">
         <v>126</v>
       </c>
       <c r="B52" s="7" t="s">
@@ -2408,7 +2408,7 @@
       <c r="K52" s="7"/>
     </row>
     <row r="53" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="32"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="7" t="s">
         <v>106</v>
       </c>
@@ -2431,7 +2431,7 @@
       <c r="K53" s="7"/>
     </row>
     <row r="54" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="32"/>
+      <c r="A54" s="30"/>
       <c r="B54" s="7" t="s">
         <v>107</v>
       </c>
@@ -2454,7 +2454,7 @@
       <c r="K54" s="7"/>
     </row>
     <row r="55" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A55" s="32"/>
+      <c r="A55" s="30"/>
       <c r="B55" s="7" t="s">
         <v>108</v>
       </c>
@@ -2477,7 +2477,7 @@
       <c r="K55" s="7"/>
     </row>
     <row r="56" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A56" s="32"/>
+      <c r="A56" s="30"/>
       <c r="B56" s="7" t="s">
         <v>109</v>
       </c>
@@ -2500,7 +2500,7 @@
       <c r="K56" s="7"/>
     </row>
     <row r="57" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A57" s="32"/>
+      <c r="A57" s="30"/>
       <c r="B57" s="7" t="s">
         <v>110</v>
       </c>
@@ -2523,7 +2523,7 @@
       <c r="K57" s="7"/>
     </row>
     <row r="58" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A58" s="32"/>
+      <c r="A58" s="30"/>
       <c r="B58" s="7" t="s">
         <v>111</v>
       </c>
@@ -2546,7 +2546,7 @@
       <c r="K58" s="7"/>
     </row>
     <row r="59" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A59" s="32"/>
+      <c r="A59" s="30"/>
       <c r="B59" s="7" t="s">
         <v>112</v>
       </c>
@@ -2569,7 +2569,7 @@
       <c r="K59" s="7"/>
     </row>
     <row r="60" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A60" s="32"/>
+      <c r="A60" s="30"/>
       <c r="B60" s="7" t="s">
         <v>113</v>
       </c>
@@ -2592,7 +2592,7 @@
       <c r="K60" s="7"/>
     </row>
     <row r="61" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A61" s="32"/>
+      <c r="A61" s="30"/>
       <c r="B61" s="7" t="s">
         <v>114</v>
       </c>
@@ -2615,7 +2615,7 @@
       <c r="K61" s="7"/>
     </row>
     <row r="62" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A62" s="32"/>
+      <c r="A62" s="30"/>
       <c r="B62" s="7" t="s">
         <v>115</v>
       </c>
@@ -2638,7 +2638,7 @@
       <c r="K62" s="7"/>
     </row>
     <row r="63" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A63" s="32"/>
+      <c r="A63" s="30"/>
       <c r="B63" s="7" t="s">
         <v>116</v>
       </c>
@@ -2661,7 +2661,7 @@
       <c r="K63" s="7"/>
     </row>
     <row r="64" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="32"/>
+      <c r="A64" s="30"/>
       <c r="B64" s="7" t="s">
         <v>117</v>
       </c>
@@ -2684,7 +2684,7 @@
       <c r="K64" s="7"/>
     </row>
     <row r="65" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="32"/>
+      <c r="A65" s="30"/>
       <c r="B65" s="7" t="s">
         <v>118</v>
       </c>
@@ -2707,7 +2707,7 @@
       <c r="K65" s="7"/>
     </row>
     <row r="66" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A66" s="39"/>
+      <c r="A66" s="31"/>
       <c r="B66" s="7" t="s">
         <v>119</v>
       </c>
@@ -2730,7 +2730,7 @@
       <c r="K66" s="7"/>
     </row>
     <row r="67" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="31" t="s">
+      <c r="A67" s="29" t="s">
         <v>138</v>
       </c>
       <c r="B67" s="7" t="s">
@@ -2755,7 +2755,7 @@
       <c r="K67" s="7"/>
     </row>
     <row r="68" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="32"/>
+      <c r="A68" s="30"/>
       <c r="B68" s="7" t="s">
         <v>129</v>
       </c>
@@ -2778,7 +2778,7 @@
       <c r="K68" s="7"/>
     </row>
     <row r="69" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="32"/>
+      <c r="A69" s="30"/>
       <c r="B69" s="7" t="s">
         <v>139</v>
       </c>
@@ -2801,8 +2801,8 @@
       <c r="K69" s="7"/>
     </row>
     <row r="70" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A70" s="32"/>
-      <c r="B70" s="40" t="s">
+      <c r="A70" s="30"/>
+      <c r="B70" s="28" t="s">
         <v>140</v>
       </c>
       <c r="C70" s="25">
@@ -2824,8 +2824,8 @@
       <c r="K70" s="7"/>
     </row>
     <row r="71" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A71" s="32"/>
-      <c r="B71" s="40" t="s">
+      <c r="A71" s="30"/>
+      <c r="B71" s="28" t="s">
         <v>141</v>
       </c>
       <c r="C71" s="25"/>
@@ -2839,8 +2839,8 @@
       <c r="K71" s="7"/>
     </row>
     <row r="72" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A72" s="32"/>
-      <c r="B72" s="40" t="s">
+      <c r="A72" s="30"/>
+      <c r="B72" s="28" t="s">
         <v>142</v>
       </c>
       <c r="C72" s="25"/>
@@ -2854,8 +2854,8 @@
       <c r="K72" s="7"/>
     </row>
     <row r="73" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A73" s="32"/>
-      <c r="B73" s="40" t="s">
+      <c r="A73" s="30"/>
+      <c r="B73" s="28" t="s">
         <v>143</v>
       </c>
       <c r="C73" s="25"/>
@@ -2869,7 +2869,7 @@
       <c r="K73" s="7"/>
     </row>
     <row r="74" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A74" s="32"/>
+      <c r="A74" s="30"/>
       <c r="B74" s="7" t="s">
         <v>130</v>
       </c>
@@ -2892,7 +2892,7 @@
       <c r="K74" s="7"/>
     </row>
     <row r="75" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A75" s="32"/>
+      <c r="A75" s="30"/>
       <c r="B75" s="7" t="s">
         <v>131</v>
       </c>
@@ -2915,7 +2915,7 @@
       <c r="K75" s="7"/>
     </row>
     <row r="76" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A76" s="32"/>
+      <c r="A76" s="30"/>
       <c r="B76" s="7" t="s">
         <v>132</v>
       </c>
@@ -2938,7 +2938,7 @@
       <c r="K76" s="7"/>
     </row>
     <row r="77" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A77" s="32"/>
+      <c r="A77" s="30"/>
       <c r="B77" s="7" t="s">
         <v>133</v>
       </c>
@@ -2961,7 +2961,7 @@
       <c r="K77" s="7"/>
     </row>
     <row r="78" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A78" s="32"/>
+      <c r="A78" s="30"/>
       <c r="B78" s="7" t="s">
         <v>134</v>
       </c>
@@ -2984,7 +2984,7 @@
       <c r="K78" s="7"/>
     </row>
     <row r="79" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="32"/>
+      <c r="A79" s="30"/>
       <c r="B79" s="7" t="s">
         <v>135</v>
       </c>
@@ -3007,7 +3007,7 @@
       <c r="K79" s="7"/>
     </row>
     <row r="80" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A80" s="32"/>
+      <c r="A80" s="30"/>
       <c r="B80" s="7" t="s">
         <v>136</v>
       </c>
@@ -3030,7 +3030,7 @@
       <c r="K80" s="7"/>
     </row>
     <row r="81" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="39"/>
+      <c r="A81" s="31"/>
       <c r="B81" s="7" t="s">
         <v>137</v>
       </c>
@@ -3385,10 +3385,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="35">
         <v>3</v>
       </c>
       <c r="C2" s="6"/>
@@ -3401,8 +3401,8 @@
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="s">
         <v>41</v>
@@ -3413,8 +3413,8 @@
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7" t="s">
         <v>42</v>
@@ -3448,108 +3448,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="38" t="s">
+      <c r="C1" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="37" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37" t="s">
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37" t="s">
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="38" t="s">
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="38"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="38"/>
-      <c r="V3" s="38"/>
-      <c r="W3" s="38"/>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="38"/>
-      <c r="Z3" s="38"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="40"/>
+      <c r="Y3" s="40"/>
+      <c r="Z3" s="40"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="12" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
automate DFWT_TC_14 and DFWT_TC_24
</commit_message>
<xml_diff>
--- a/DFWT Change Request Update.xlsx
+++ b/DFWT Change Request Update.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="153">
   <si>
     <t>Change Request #</t>
   </si>
@@ -535,6 +535,21 @@
   </si>
   <si>
     <t>Verify upon creating a new project, success notification dialog will appear and the project will be created.</t>
+  </si>
+  <si>
+    <t>Automated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify the expand functionalities of all parent folder to expand its subtree(if any), and all its succeding folder (if any) </t>
+  </si>
+  <si>
+    <t>DFWT_TC_23</t>
+  </si>
+  <si>
+    <t>DFWT_TC_24</t>
+  </si>
+  <si>
+    <t>Verify when deleting a Project, a success notification dialog will appear saying "&lt;projectName&gt; project has been successfully deleted."</t>
   </si>
 </sst>
 </file>
@@ -709,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -784,36 +799,42 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -837,6 +858,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1139,19 +1163,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K110"/>
+  <dimension ref="A1:K111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.26953125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="53.26953125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.81640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9" style="4" customWidth="1"/>
+    <col min="2" max="2" width="46.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.54296875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15" style="2" customWidth="1"/>
     <col min="6" max="6" width="22.26953125" style="2" customWidth="1"/>
     <col min="7" max="7" width="21" style="2" customWidth="1"/>
     <col min="8" max="8" width="17.7265625" style="2" customWidth="1"/>
@@ -1411,7 +1435,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
@@ -1492,7 +1516,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>62</v>
       </c>
@@ -1519,7 +1543,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>63</v>
       </c>
@@ -1546,43 +1570,47 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" ht="31" x14ac:dyDescent="0.35">
-      <c r="A15" s="32" t="s">
+    <row r="15" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="31" t="s">
         <v>69</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="28">
         <v>43970</v>
       </c>
       <c r="D15" s="23"/>
-      <c r="E15" s="29">
+      <c r="E15" s="28">
         <v>43970</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="9"/>
+      <c r="F15" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>29</v>
+      </c>
       <c r="H15" s="9"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="34"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="C16" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="29">
+      <c r="C16" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="28">
         <v>43970</v>
       </c>
-      <c r="F16" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="28" t="s">
+      <c r="F16" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="G16" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H16" s="7"/>
@@ -1591,19 +1619,21 @@
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="34"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C17" s="29">
+      <c r="C17" s="28">
         <v>43970</v>
       </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="29">
+      <c r="D17" s="30"/>
+      <c r="E17" s="28">
         <v>43970</v>
       </c>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28" t="s">
+      <c r="F17" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="G17" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H17" s="7"/>
@@ -1612,19 +1642,21 @@
       <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="34"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C18" s="29">
+      <c r="C18" s="28">
         <v>43970</v>
       </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="29">
+      <c r="D18" s="30"/>
+      <c r="E18" s="28">
         <v>43970</v>
       </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28" t="s">
+      <c r="F18" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="G18" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H18" s="7"/>
@@ -1633,19 +1665,23 @@
       <c r="K18" s="7"/>
     </row>
     <row r="19" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="33"/>
+      <c r="A19" s="31" t="s">
+        <v>151</v>
+      </c>
       <c r="B19" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="C19" s="29">
+      <c r="C19" s="28">
         <v>43969</v>
       </c>
-      <c r="D19" s="31"/>
-      <c r="E19" s="29">
+      <c r="D19" s="30"/>
+      <c r="E19" s="28">
         <v>43970</v>
       </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28" t="s">
+      <c r="F19" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="G19" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H19" s="7"/>
@@ -1653,24 +1689,22 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D20" s="31"/>
-      <c r="E20" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="28" t="s">
+    <row r="20" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="33"/>
+      <c r="B20" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C20" s="28">
+        <v>43970</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="28">
+        <v>43970</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="G20" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H20" s="7"/>
@@ -1679,21 +1713,23 @@
       <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="35"/>
+      <c r="A21" s="37" t="s">
+        <v>70</v>
+      </c>
       <c r="B21" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D21" s="31"/>
-      <c r="E21" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G21" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D21" s="30"/>
+      <c r="E21" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H21" s="7"/>
@@ -1701,22 +1737,22 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="35"/>
-      <c r="B22" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C22" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D22" s="31"/>
-      <c r="E22" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G22" s="28" t="s">
+    <row r="22" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="37"/>
+      <c r="B22" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D22" s="30"/>
+      <c r="E22" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H22" s="7"/>
@@ -1724,24 +1760,22 @@
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D23" s="31"/>
-      <c r="E23" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F23" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23" s="28" t="s">
+    <row r="23" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="37"/>
+      <c r="B23" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D23" s="30"/>
+      <c r="E23" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H23" s="7"/>
@@ -1749,24 +1783,24 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="36" t="s">
-        <v>72</v>
+    <row r="24" spans="1:11" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="20" t="s">
+        <v>71</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D24" s="31"/>
-      <c r="E24" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F24" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G24" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D24" s="30"/>
+      <c r="E24" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H24" s="7"/>
@@ -1774,22 +1808,24 @@
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="37"/>
+    <row r="25" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="38" t="s">
+        <v>72</v>
+      </c>
       <c r="B25" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D25" s="31"/>
-      <c r="E25" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F25" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G25" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D25" s="30"/>
+      <c r="E25" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H25" s="7"/>
@@ -1797,24 +1833,22 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="20" t="s">
-        <v>73</v>
-      </c>
+    <row r="26" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A26" s="39"/>
       <c r="B26" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D26" s="31"/>
-      <c r="E26" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G26" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D26" s="30"/>
+      <c r="E26" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H26" s="7"/>
@@ -1822,24 +1856,24 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="32" t="s">
-        <v>88</v>
+    <row r="27" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="20" t="s">
+        <v>73</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D27" s="31"/>
-      <c r="E27" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F27" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G27" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D27" s="30"/>
+      <c r="E27" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H27" s="7"/>
@@ -1847,22 +1881,24 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="34"/>
+    <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="34" t="s">
+        <v>88</v>
+      </c>
       <c r="B28" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C28" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D28" s="31"/>
-      <c r="E28" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F28" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G28" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D28" s="30"/>
+      <c r="E28" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H28" s="7"/>
@@ -1870,22 +1906,22 @@
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="34"/>
+    <row r="29" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="35"/>
       <c r="B29" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D29" s="31"/>
-      <c r="E29" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F29" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G29" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D29" s="30"/>
+      <c r="E29" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H29" s="7"/>
@@ -1893,22 +1929,22 @@
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30" s="34"/>
+    <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="35"/>
       <c r="B30" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D30" s="31"/>
-      <c r="E30" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F30" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G30" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D30" s="30"/>
+      <c r="E30" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H30" s="7"/>
@@ -1916,22 +1952,22 @@
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31" s="34"/>
+    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="35"/>
       <c r="B31" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G31" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D31" s="30"/>
+      <c r="E31" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H31" s="7"/>
@@ -1940,21 +1976,21 @@
       <c r="K31" s="7"/>
     </row>
     <row r="32" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="34"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D32" s="31"/>
-      <c r="E32" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F32" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G32" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D32" s="30"/>
+      <c r="E32" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F32" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H32" s="7"/>
@@ -1962,22 +1998,22 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="34"/>
+    <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="35"/>
       <c r="B33" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D33" s="31"/>
-      <c r="E33" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F33" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G33" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D33" s="30"/>
+      <c r="E33" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H33" s="7"/>
@@ -1985,22 +2021,22 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="34"/>
+    <row r="34" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A34" s="35"/>
       <c r="B34" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D34" s="31"/>
-      <c r="E34" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F34" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G34" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D34" s="30"/>
+      <c r="E34" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F34" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G34" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H34" s="7"/>
@@ -2008,24 +2044,22 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="32" t="s">
-        <v>101</v>
-      </c>
+    <row r="35" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="35"/>
       <c r="B35" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D35" s="31"/>
-      <c r="E35" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F35" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G35" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D35" s="30"/>
+      <c r="E35" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H35" s="7"/>
@@ -2033,22 +2067,24 @@
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="34"/>
+    <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="34" t="s">
+        <v>101</v>
+      </c>
       <c r="B36" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D36" s="31"/>
-      <c r="E36" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F36" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G36" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D36" s="30"/>
+      <c r="E36" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H36" s="7"/>
@@ -2056,22 +2092,22 @@
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="34"/>
+    <row r="37" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="35"/>
       <c r="B37" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D37" s="31"/>
-      <c r="E37" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F37" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G37" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D37" s="30"/>
+      <c r="E37" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H37" s="7"/>
@@ -2079,22 +2115,22 @@
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="34"/>
+    <row r="38" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="35"/>
       <c r="B38" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D38" s="31"/>
-      <c r="E38" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F38" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G38" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D38" s="30"/>
+      <c r="E38" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H38" s="7"/>
@@ -2102,22 +2138,22 @@
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="34"/>
+    <row r="39" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="35"/>
       <c r="B39" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C39" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D39" s="31"/>
-      <c r="E39" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F39" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G39" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D39" s="30"/>
+      <c r="E39" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F39" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H39" s="7"/>
@@ -2126,21 +2162,21 @@
       <c r="K39" s="7"/>
     </row>
     <row r="40" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="34"/>
+      <c r="A40" s="35"/>
       <c r="B40" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C40" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D40" s="31"/>
-      <c r="E40" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F40" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G40" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D40" s="30"/>
+      <c r="E40" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F40" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H40" s="7"/>
@@ -2148,22 +2184,22 @@
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="34"/>
+    <row r="41" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="35"/>
       <c r="B41" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D41" s="31"/>
-      <c r="E41" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F41" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G41" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D41" s="30"/>
+      <c r="E41" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F41" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G41" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H41" s="7"/>
@@ -2171,22 +2207,22 @@
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="34"/>
+    <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="35"/>
       <c r="B42" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C42" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D42" s="31"/>
-      <c r="E42" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F42" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G42" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D42" s="30"/>
+      <c r="E42" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F42" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H42" s="7"/>
@@ -2194,22 +2230,22 @@
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="34"/>
+    <row r="43" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="35"/>
       <c r="B43" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C43" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D43" s="31"/>
-      <c r="E43" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F43" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G43" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D43" s="30"/>
+      <c r="E43" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F43" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G43" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H43" s="7"/>
@@ -2218,21 +2254,21 @@
       <c r="K43" s="7"/>
     </row>
     <row r="44" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="34"/>
+      <c r="A44" s="35"/>
       <c r="B44" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C44" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D44" s="31"/>
-      <c r="E44" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F44" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G44" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D44" s="30"/>
+      <c r="E44" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F44" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H44" s="7"/>
@@ -2240,22 +2276,22 @@
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
     </row>
-    <row r="45" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="34"/>
+    <row r="45" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="35"/>
       <c r="B45" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C45" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D45" s="31"/>
-      <c r="E45" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F45" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G45" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D45" s="30"/>
+      <c r="E45" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F45" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H45" s="7"/>
@@ -2264,21 +2300,21 @@
       <c r="K45" s="7"/>
     </row>
     <row r="46" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="34"/>
+      <c r="A46" s="35"/>
       <c r="B46" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C46" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D46" s="31"/>
-      <c r="E46" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F46" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G46" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D46" s="30"/>
+      <c r="E46" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F46" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G46" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H46" s="7"/>
@@ -2287,21 +2323,21 @@
       <c r="K46" s="7"/>
     </row>
     <row r="47" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="34"/>
+      <c r="A47" s="35"/>
       <c r="B47" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D47" s="31"/>
-      <c r="E47" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F47" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G47" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D47" s="30"/>
+      <c r="E47" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F47" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G47" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H47" s="7"/>
@@ -2310,21 +2346,21 @@
       <c r="K47" s="7"/>
     </row>
     <row r="48" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="34"/>
+      <c r="A48" s="35"/>
       <c r="B48" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C48" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D48" s="31"/>
-      <c r="E48" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F48" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G48" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D48" s="30"/>
+      <c r="E48" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F48" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G48" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H48" s="7"/>
@@ -2333,21 +2369,21 @@
       <c r="K48" s="7"/>
     </row>
     <row r="49" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="34"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C49" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D49" s="31"/>
-      <c r="E49" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F49" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G49" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D49" s="30"/>
+      <c r="E49" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F49" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G49" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H49" s="7"/>
@@ -2356,21 +2392,21 @@
       <c r="K49" s="7"/>
     </row>
     <row r="50" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="34"/>
+      <c r="A50" s="35"/>
       <c r="B50" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C50" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D50" s="31"/>
-      <c r="E50" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F50" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G50" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D50" s="30"/>
+      <c r="E50" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F50" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G50" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H50" s="7"/>
@@ -2379,21 +2415,21 @@
       <c r="K50" s="7"/>
     </row>
     <row r="51" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A51" s="34"/>
+      <c r="A51" s="35"/>
       <c r="B51" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C51" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D51" s="31"/>
-      <c r="E51" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F51" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G51" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D51" s="30"/>
+      <c r="E51" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F51" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G51" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H51" s="7"/>
@@ -2401,22 +2437,22 @@
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
     </row>
-    <row r="52" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="34"/>
+    <row r="52" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A52" s="35"/>
       <c r="B52" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C52" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D52" s="31"/>
-      <c r="E52" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F52" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G52" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C52" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D52" s="30"/>
+      <c r="E52" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F52" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G52" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H52" s="7"/>
@@ -2424,22 +2460,22 @@
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
     </row>
-    <row r="53" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="34"/>
+    <row r="53" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A53" s="35"/>
       <c r="B53" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C53" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D53" s="31"/>
-      <c r="E53" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F53" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G53" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C53" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D53" s="30"/>
+      <c r="E53" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F53" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G53" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H53" s="7"/>
@@ -2447,22 +2483,22 @@
       <c r="J53" s="7"/>
       <c r="K53" s="7"/>
     </row>
-    <row r="54" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="34"/>
+    <row r="54" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A54" s="35"/>
       <c r="B54" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="C54" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D54" s="31"/>
-      <c r="E54" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F54" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G54" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D54" s="30"/>
+      <c r="E54" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F54" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G54" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H54" s="7"/>
@@ -2470,22 +2506,22 @@
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
     </row>
-    <row r="55" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="33"/>
+    <row r="55" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A55" s="35"/>
       <c r="B55" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C55" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D55" s="31"/>
-      <c r="E55" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F55" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G55" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C55" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D55" s="30"/>
+      <c r="E55" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F55" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G55" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H55" s="7"/>
@@ -2494,23 +2530,21 @@
       <c r="K55" s="7"/>
     </row>
     <row r="56" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A56" s="32" t="s">
-        <v>125</v>
-      </c>
+      <c r="A56" s="36"/>
       <c r="B56" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="C56" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D56" s="31"/>
-      <c r="E56" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F56" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G56" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D56" s="30"/>
+      <c r="E56" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F56" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G56" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H56" s="7"/>
@@ -2518,22 +2552,24 @@
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
     </row>
-    <row r="57" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="34"/>
+    <row r="57" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A57" s="34" t="s">
+        <v>125</v>
+      </c>
       <c r="B57" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C57" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D57" s="31"/>
-      <c r="E57" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F57" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G57" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D57" s="30"/>
+      <c r="E57" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F57" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G57" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H57" s="7"/>
@@ -2542,21 +2578,21 @@
       <c r="K57" s="7"/>
     </row>
     <row r="58" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="34"/>
+      <c r="A58" s="35"/>
       <c r="B58" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C58" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D58" s="31"/>
-      <c r="E58" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F58" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G58" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C58" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D58" s="30"/>
+      <c r="E58" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F58" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G58" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H58" s="7"/>
@@ -2564,22 +2600,22 @@
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
     </row>
-    <row r="59" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A59" s="34"/>
+    <row r="59" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A59" s="35"/>
       <c r="B59" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C59" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D59" s="31"/>
-      <c r="E59" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F59" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G59" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D59" s="30"/>
+      <c r="E59" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F59" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G59" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H59" s="7"/>
@@ -2587,22 +2623,22 @@
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
     </row>
-    <row r="60" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A60" s="34"/>
+    <row r="60" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A60" s="35"/>
       <c r="B60" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C60" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D60" s="31"/>
-      <c r="E60" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F60" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G60" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D60" s="30"/>
+      <c r="E60" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F60" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G60" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H60" s="7"/>
@@ -2610,22 +2646,22 @@
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
     </row>
-    <row r="61" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A61" s="34"/>
+    <row r="61" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="35"/>
       <c r="B61" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C61" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D61" s="31"/>
-      <c r="E61" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F61" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G61" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C61" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D61" s="30"/>
+      <c r="E61" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F61" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G61" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H61" s="7"/>
@@ -2634,21 +2670,21 @@
       <c r="K61" s="7"/>
     </row>
     <row r="62" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A62" s="34"/>
+      <c r="A62" s="35"/>
       <c r="B62" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C62" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D62" s="31"/>
-      <c r="E62" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F62" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G62" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D62" s="30"/>
+      <c r="E62" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F62" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G62" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H62" s="7"/>
@@ -2657,21 +2693,21 @@
       <c r="K62" s="7"/>
     </row>
     <row r="63" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A63" s="34"/>
+      <c r="A63" s="35"/>
       <c r="B63" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C63" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D63" s="31"/>
-      <c r="E63" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F63" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G63" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D63" s="30"/>
+      <c r="E63" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F63" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G63" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H63" s="7"/>
@@ -2679,22 +2715,22 @@
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
     </row>
-    <row r="64" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A64" s="34"/>
+    <row r="64" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A64" s="35"/>
       <c r="B64" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C64" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D64" s="31"/>
-      <c r="E64" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F64" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G64" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="C64" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D64" s="30"/>
+      <c r="E64" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F64" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G64" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H64" s="7"/>
@@ -2703,21 +2739,21 @@
       <c r="K64" s="7"/>
     </row>
     <row r="65" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A65" s="34"/>
+      <c r="A65" s="35"/>
       <c r="B65" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C65" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D65" s="31"/>
-      <c r="E65" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F65" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G65" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D65" s="30"/>
+      <c r="E65" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F65" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G65" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H65" s="7"/>
@@ -2726,21 +2762,21 @@
       <c r="K65" s="7"/>
     </row>
     <row r="66" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="34"/>
+      <c r="A66" s="35"/>
       <c r="B66" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C66" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D66" s="31"/>
-      <c r="E66" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F66" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G66" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C66" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D66" s="30"/>
+      <c r="E66" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F66" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G66" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H66" s="7"/>
@@ -2748,22 +2784,22 @@
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
     </row>
-    <row r="67" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="34"/>
+    <row r="67" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="35"/>
       <c r="B67" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C67" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D67" s="31"/>
-      <c r="E67" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F67" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G67" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C67" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D67" s="30"/>
+      <c r="E67" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F67" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G67" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H67" s="7"/>
@@ -2772,21 +2808,21 @@
       <c r="K67" s="7"/>
     </row>
     <row r="68" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" s="34"/>
+      <c r="A68" s="35"/>
       <c r="B68" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C68" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D68" s="31"/>
-      <c r="E68" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F68" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G68" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C68" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D68" s="30"/>
+      <c r="E68" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F68" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G68" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H68" s="7"/>
@@ -2795,21 +2831,21 @@
       <c r="K68" s="7"/>
     </row>
     <row r="69" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="34"/>
+      <c r="A69" s="35"/>
       <c r="B69" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C69" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D69" s="31"/>
-      <c r="E69" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F69" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G69" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C69" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D69" s="30"/>
+      <c r="E69" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F69" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G69" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H69" s="7"/>
@@ -2817,22 +2853,22 @@
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
     </row>
-    <row r="70" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A70" s="33"/>
+    <row r="70" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A70" s="35"/>
       <c r="B70" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C70" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D70" s="31"/>
-      <c r="E70" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F70" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G70" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C70" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D70" s="30"/>
+      <c r="E70" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F70" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G70" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H70" s="7"/>
@@ -2840,24 +2876,22 @@
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
     </row>
-    <row r="71" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A71" s="32" t="s">
-        <v>137</v>
-      </c>
+    <row r="71" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A71" s="36"/>
       <c r="B71" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C71" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D71" s="31"/>
-      <c r="E71" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F71" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G71" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C71" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D71" s="30"/>
+      <c r="E71" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F71" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G71" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H71" s="7"/>
@@ -2866,21 +2900,23 @@
       <c r="K71" s="7"/>
     </row>
     <row r="72" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A72" s="34"/>
+      <c r="A72" s="34" t="s">
+        <v>137</v>
+      </c>
       <c r="B72" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C72" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D72" s="31"/>
-      <c r="E72" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F72" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G72" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C72" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D72" s="30"/>
+      <c r="E72" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F72" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G72" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H72" s="7"/>
@@ -2889,21 +2925,21 @@
       <c r="K72" s="7"/>
     </row>
     <row r="73" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A73" s="34"/>
+      <c r="A73" s="35"/>
       <c r="B73" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C73" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D73" s="31"/>
-      <c r="E73" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F73" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G73" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="C73" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D73" s="30"/>
+      <c r="E73" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F73" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G73" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H73" s="7"/>
@@ -2911,22 +2947,22 @@
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
     </row>
-    <row r="74" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A74" s="34"/>
-      <c r="B74" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="C74" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D74" s="31"/>
-      <c r="E74" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F74" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G74" s="28" t="s">
+    <row r="74" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A74" s="35"/>
+      <c r="B74" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C74" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D74" s="30"/>
+      <c r="E74" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F74" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G74" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H74" s="7"/>
@@ -2934,102 +2970,102 @@
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
     </row>
-    <row r="75" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="34"/>
+    <row r="75" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="35"/>
       <c r="B75" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="C75" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D75" s="31"/>
-      <c r="E75" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F75" s="27"/>
-      <c r="G75" s="28"/>
+        <v>139</v>
+      </c>
+      <c r="C75" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D75" s="30"/>
+      <c r="E75" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F75" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G75" s="27" t="s">
+        <v>29</v>
+      </c>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
     </row>
     <row r="76" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="34"/>
+      <c r="A76" s="35"/>
       <c r="B76" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="C76" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D76" s="31"/>
-      <c r="E76" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F76" s="27"/>
-      <c r="G76" s="28"/>
+        <v>140</v>
+      </c>
+      <c r="C76" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D76" s="30"/>
+      <c r="E76" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F76" s="26"/>
+      <c r="G76" s="27"/>
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
     </row>
-    <row r="77" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A77" s="34"/>
+    <row r="77" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A77" s="35"/>
       <c r="B77" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="C77" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D77" s="31"/>
-      <c r="E77" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F77" s="27"/>
-      <c r="G77" s="28"/>
+        <v>141</v>
+      </c>
+      <c r="C77" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D77" s="30"/>
+      <c r="E77" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F77" s="26"/>
+      <c r="G77" s="27"/>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
     </row>
     <row r="78" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A78" s="34"/>
-      <c r="B78" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C78" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D78" s="31"/>
-      <c r="E78" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F78" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G78" s="28" t="s">
-        <v>29</v>
-      </c>
+      <c r="A78" s="35"/>
+      <c r="B78" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="C78" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D78" s="30"/>
+      <c r="E78" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F78" s="26"/>
+      <c r="G78" s="27"/>
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
     </row>
     <row r="79" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="34"/>
+      <c r="A79" s="35"/>
       <c r="B79" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C79" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D79" s="31"/>
-      <c r="E79" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F79" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G79" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="C79" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D79" s="30"/>
+      <c r="E79" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F79" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G79" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H79" s="7"/>
@@ -3038,21 +3074,21 @@
       <c r="K79" s="7"/>
     </row>
     <row r="80" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="34"/>
+      <c r="A80" s="35"/>
       <c r="B80" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C80" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D80" s="31"/>
-      <c r="E80" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F80" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G80" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="C80" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D80" s="30"/>
+      <c r="E80" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F80" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G80" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H80" s="7"/>
@@ -3060,22 +3096,22 @@
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
     </row>
-    <row r="81" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="34"/>
+    <row r="81" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A81" s="35"/>
       <c r="B81" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C81" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D81" s="31"/>
-      <c r="E81" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F81" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G81" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C81" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D81" s="30"/>
+      <c r="E81" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F81" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G81" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H81" s="7"/>
@@ -3083,22 +3119,22 @@
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
     </row>
-    <row r="82" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A82" s="34"/>
+    <row r="82" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A82" s="35"/>
       <c r="B82" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C82" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D82" s="31"/>
-      <c r="E82" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F82" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G82" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C82" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D82" s="30"/>
+      <c r="E82" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F82" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G82" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H82" s="7"/>
@@ -3106,22 +3142,22 @@
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
     </row>
-    <row r="83" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="34"/>
+    <row r="83" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A83" s="35"/>
       <c r="B83" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C83" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D83" s="31"/>
-      <c r="E83" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F83" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G83" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C83" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D83" s="30"/>
+      <c r="E83" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F83" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G83" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H83" s="7"/>
@@ -3129,22 +3165,22 @@
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
     </row>
-    <row r="84" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="34"/>
+    <row r="84" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A84" s="35"/>
       <c r="B84" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C84" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D84" s="31"/>
-      <c r="E84" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F84" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G84" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="C84" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D84" s="30"/>
+      <c r="E84" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F84" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G84" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H84" s="7"/>
@@ -3152,22 +3188,22 @@
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
     </row>
-    <row r="85" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A85" s="33"/>
+    <row r="85" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A85" s="35"/>
       <c r="B85" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C85" s="30">
-        <v>43966</v>
-      </c>
-      <c r="D85" s="31"/>
-      <c r="E85" s="30">
-        <v>43966</v>
-      </c>
-      <c r="F85" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="G85" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C85" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D85" s="30"/>
+      <c r="E85" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F85" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G85" s="27" t="s">
         <v>29</v>
       </c>
       <c r="H85" s="7"/>
@@ -3175,23 +3211,39 @@
       <c r="J85" s="7"/>
       <c r="K85" s="7"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A86" s="22"/>
-      <c r="B86" s="7"/>
-      <c r="C86" s="7"/>
-      <c r="D86" s="7"/>
-      <c r="E86" s="7"/>
-      <c r="F86" s="7"/>
-      <c r="G86" s="7"/>
+    <row r="86" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A86" s="36"/>
+      <c r="B86" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C86" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D86" s="30"/>
+      <c r="E86" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F86" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G86" s="27" t="s">
+        <v>29</v>
+      </c>
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
       <c r="K86" s="7"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A87" s="22"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
+    <row r="87" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A87" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C87" s="28">
+        <v>43970</v>
+      </c>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
@@ -3202,7 +3254,7 @@
       <c r="K87" s="7"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A88" s="22"/>
+      <c r="A88" s="21"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
@@ -3215,7 +3267,7 @@
       <c r="K88" s="7"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A89" s="22"/>
+      <c r="A89" s="21"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
@@ -3228,7 +3280,7 @@
       <c r="K89" s="7"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A90" s="22"/>
+      <c r="A90" s="21"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
@@ -3241,7 +3293,7 @@
       <c r="K90" s="7"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A91" s="22"/>
+      <c r="A91" s="21"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
@@ -3254,7 +3306,7 @@
       <c r="K91" s="7"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A92" s="22"/>
+      <c r="A92" s="21"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
@@ -3267,7 +3319,7 @@
       <c r="K92" s="7"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A93" s="22"/>
+      <c r="A93" s="21"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
@@ -3280,7 +3332,7 @@
       <c r="K93" s="7"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A94" s="22"/>
+      <c r="A94" s="21"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
@@ -3293,7 +3345,7 @@
       <c r="K94" s="7"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A95" s="22"/>
+      <c r="A95" s="21"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
@@ -3306,7 +3358,7 @@
       <c r="K95" s="7"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A96" s="22"/>
+      <c r="A96" s="21"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
@@ -3319,7 +3371,7 @@
       <c r="K96" s="7"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A97" s="22"/>
+      <c r="A97" s="21"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
@@ -3332,7 +3384,7 @@
       <c r="K97" s="7"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A98" s="22"/>
+      <c r="A98" s="21"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
@@ -3345,7 +3397,7 @@
       <c r="K98" s="7"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A99" s="22"/>
+      <c r="A99" s="21"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
@@ -3358,7 +3410,7 @@
       <c r="K99" s="7"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A100" s="22"/>
+      <c r="A100" s="21"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
@@ -3371,7 +3423,7 @@
       <c r="K100" s="7"/>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A101" s="22"/>
+      <c r="A101" s="19"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
@@ -3410,7 +3462,7 @@
       <c r="K103" s="7"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A104" s="21"/>
+      <c r="A104" s="22"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
@@ -3423,7 +3475,7 @@
       <c r="K104" s="7"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A105" s="19"/>
+      <c r="A105" s="21"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
@@ -3435,35 +3487,49 @@
       <c r="J105" s="7"/>
       <c r="K105" s="7"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A107" s="5" t="s">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A106" s="19"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="7"/>
+      <c r="E106" s="7"/>
+      <c r="F106" s="7"/>
+      <c r="G106" s="7"/>
+      <c r="H106" s="7"/>
+      <c r="I106" s="7"/>
+      <c r="J106" s="7"/>
+      <c r="K106" s="7"/>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A108" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A108" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A109" s="10" t="s">
+      <c r="A109" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A110" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A110" s="11" t="s">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A111" s="11" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A71:A85"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A27:A34"/>
-    <mergeCell ref="A56:A70"/>
-    <mergeCell ref="A35:A55"/>
-    <mergeCell ref="A15:A19"/>
+  <mergeCells count="8">
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A72:A86"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="A57:A71"/>
+    <mergeCell ref="A36:A56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3509,10 +3575,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="40">
         <v>3</v>
       </c>
       <c r="C2" s="6"/>
@@ -3525,8 +3591,8 @@
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="s">
         <v>41</v>
@@ -3537,8 +3603,8 @@
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7" t="s">
         <v>42</v>
@@ -3572,108 +3638,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="43" t="s">
+      <c r="C1" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="42" t="s">
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42" t="s">
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="42"/>
-      <c r="S2" s="42"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="43" t="s">
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
+      <c r="V2" s="45"/>
+      <c r="W2" s="45"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="45"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="43"/>
-      <c r="X3" s="43"/>
-      <c r="Y3" s="43"/>
-      <c r="Z3" s="43"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="44"/>
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="44"/>
+      <c r="T3" s="44"/>
+      <c r="U3" s="45"/>
+      <c r="V3" s="45"/>
+      <c r="W3" s="45"/>
+      <c r="X3" s="45"/>
+      <c r="Y3" s="45"/>
+      <c r="Z3" s="45"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="12" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
automate DFWT_TC_16, enhanced DFWT_TC_15, to be continue DFWT_TC_17
</commit_message>
<xml_diff>
--- a/DFWT Change Request Update.xlsx
+++ b/DFWT Change Request Update.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="155">
   <si>
     <t>Change Request #</t>
   </si>
@@ -273,9 +273,6 @@
     <t>Verify if a user clicks “Add to Group” then it should move a specific Die Revision/Bank to the selected Group.</t>
   </si>
   <si>
-    <t>After creating a Team Members, a dialog will popup that says "&lt;Name&gt;  was successfully added as a project member."</t>
-  </si>
-  <si>
     <t>DFWT_TC_14</t>
   </si>
   <si>
@@ -301,9 +298,6 @@
   </si>
   <si>
     <t>Verify if clicking Add Group Follower, "ADD SIGNOFF GROUP" dialog will pop up.</t>
-  </si>
-  <si>
-    <t>Verify if Team Member function can only exist once per project. If a user adds a new team member where a function was already assigned to someone, an alert dialog will pop up that says "&lt;functionName&gt; function is already assigned to a user. Please enter a new user or new function."</t>
   </si>
   <si>
     <t>Verify upon creating a pool, a notification will pop up if the Pool name already exist. Otherwise a successful notification will pop up.</t>
@@ -553,6 +547,15 @@
   </si>
   <si>
     <t>Verify if clicking a trash bin icon to delete Project member, Delete Confirmation dialog will pop up.</t>
+  </si>
+  <si>
+    <t>After creating a Team Members, Success Notification dialog will pop up."</t>
+  </si>
+  <si>
+    <t>Verify if an alert dialog will pop up if the function can only exist once per project. If a user adds a new team member where a function was already assigned to someone, an alert dialog will pop up that says "&lt;functionName&gt; function is already assigned to a user. Please enter a new user or new function."</t>
+  </si>
+  <si>
+    <t>Verify if an alert dialog will pop up if Employee ID is invalid saying "Invalid user information. Please input a valid user information."</t>
   </si>
 </sst>
 </file>
@@ -727,7 +730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -820,6 +823,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -864,12 +876,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1172,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K112"/>
+  <dimension ref="A1:K113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1580,11 +1586,11 @@
       <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>143</v>
+      <c r="A15" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>141</v>
       </c>
       <c r="C15" s="28">
         <v>43970</v>
@@ -1594,7 +1600,7 @@
         <v>43970</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G15" s="27" t="s">
         <v>29</v>
@@ -1605,9 +1611,9 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="33"/>
-      <c r="B16" s="8" t="s">
-        <v>146</v>
+      <c r="A16" s="36"/>
+      <c r="B16" s="34" t="s">
+        <v>144</v>
       </c>
       <c r="C16" s="29">
         <v>43966</v>
@@ -1617,7 +1623,7 @@
         <v>43970</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G16" s="27" t="s">
         <v>29</v>
@@ -1628,9 +1634,9 @@
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="33"/>
-      <c r="B17" s="8" t="s">
-        <v>144</v>
+      <c r="A17" s="36"/>
+      <c r="B17" s="34" t="s">
+        <v>142</v>
       </c>
       <c r="C17" s="28">
         <v>43970</v>
@@ -1640,7 +1646,7 @@
         <v>43970</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G17" s="27" t="s">
         <v>29</v>
@@ -1651,9 +1657,9 @@
       <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="33"/>
-      <c r="B18" s="8" t="s">
-        <v>145</v>
+      <c r="A18" s="36"/>
+      <c r="B18" s="34" t="s">
+        <v>143</v>
       </c>
       <c r="C18" s="28">
         <v>43970</v>
@@ -1663,7 +1669,7 @@
         <v>43970</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G18" s="27" t="s">
         <v>29</v>
@@ -1674,11 +1680,11 @@
       <c r="K18" s="7"/>
     </row>
     <row r="19" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>142</v>
+      <c r="A19" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>140</v>
       </c>
       <c r="C19" s="28">
         <v>43969</v>
@@ -1688,7 +1694,7 @@
         <v>43970</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G19" s="27" t="s">
         <v>29</v>
@@ -1699,9 +1705,9 @@
       <c r="K19" s="7"/>
     </row>
     <row r="20" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="34"/>
-      <c r="B20" s="8" t="s">
-        <v>151</v>
+      <c r="A20" s="37"/>
+      <c r="B20" s="34" t="s">
+        <v>149</v>
       </c>
       <c r="C20" s="28">
         <v>43970</v>
@@ -1711,7 +1717,7 @@
         <v>43970</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G20" s="27" t="s">
         <v>29</v>
@@ -1722,11 +1728,11 @@
       <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="47" t="s">
-        <v>74</v>
+      <c r="A21" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>73</v>
       </c>
       <c r="C21" s="29">
         <v>43966</v>
@@ -1746,10 +1752,10 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="38"/>
-      <c r="B22" s="47" t="s">
-        <v>152</v>
+    <row r="22" spans="1:11" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="41"/>
+      <c r="B22" s="32" t="s">
+        <v>150</v>
       </c>
       <c r="C22" s="28">
         <v>43970</v>
@@ -1765,65 +1771,55 @@
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="38"/>
-      <c r="B23" s="47" t="s">
-        <v>68</v>
+    <row r="23" spans="1:11" ht="95.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="41"/>
+      <c r="B23" s="32" t="s">
+        <v>153</v>
       </c>
       <c r="C23" s="29">
         <v>43966</v>
       </c>
       <c r="D23" s="30"/>
       <c r="E23" s="28">
-        <v>43970</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23" s="27" t="s">
-        <v>29</v>
-      </c>
+        <v>43971</v>
+      </c>
+      <c r="F23" s="26"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="38"/>
-      <c r="B24" s="48" t="s">
-        <v>153</v>
-      </c>
-      <c r="C24" s="29">
-        <v>43966</v>
+    <row r="24" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="41"/>
+      <c r="B24" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="C24" s="28">
+        <v>43971</v>
       </c>
       <c r="D24" s="30"/>
       <c r="E24" s="28">
         <v>43971</v>
       </c>
-      <c r="F24" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="G24" s="27" t="s">
-        <v>29</v>
-      </c>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>78</v>
+    <row r="25" spans="1:11" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="41"/>
+      <c r="B25" s="32" t="s">
+        <v>152</v>
       </c>
       <c r="C25" s="29">
         <v>43966</v>
       </c>
       <c r="D25" s="30"/>
-      <c r="E25" s="29">
-        <v>43966</v>
+      <c r="E25" s="28">
+        <v>43970</v>
       </c>
       <c r="F25" s="26" t="s">
         <v>27</v>
@@ -1836,19 +1832,19 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>75</v>
+    <row r="26" spans="1:11" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>151</v>
       </c>
       <c r="C26" s="29">
         <v>43966</v>
       </c>
       <c r="D26" s="30"/>
-      <c r="E26" s="29">
-        <v>43966</v>
+      <c r="E26" s="28">
+        <v>43971</v>
       </c>
       <c r="F26" s="26" t="s">
         <v>27</v>
@@ -1861,10 +1857,12 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="40"/>
+    <row r="27" spans="1:11" ht="46" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="42" t="s">
+        <v>71</v>
+      </c>
       <c r="B27" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C27" s="29">
         <v>43966</v>
@@ -1884,12 +1882,10 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="20" t="s">
-        <v>73</v>
-      </c>
+    <row r="28" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A28" s="43"/>
       <c r="B28" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C28" s="29">
         <v>43966</v>
@@ -1909,12 +1905,12 @@
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="35" t="s">
-        <v>88</v>
+    <row r="29" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="20" t="s">
+        <v>72</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C29" s="29">
         <v>43966</v>
@@ -1934,10 +1930,12 @@
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="36"/>
+    <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="38" t="s">
+        <v>86</v>
+      </c>
       <c r="B30" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C30" s="29">
         <v>43966</v>
@@ -1957,10 +1955,10 @@
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="36"/>
+    <row r="31" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="39"/>
       <c r="B31" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C31" s="29">
         <v>43966</v>
@@ -1981,9 +1979,9 @@
       <c r="K31" s="7"/>
     </row>
     <row r="32" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="36"/>
+      <c r="A32" s="39"/>
       <c r="B32" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C32" s="29">
         <v>43966</v>
@@ -2003,10 +2001,10 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="36"/>
+    <row r="33" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="39"/>
       <c r="B33" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C33" s="29">
         <v>43966</v>
@@ -2027,9 +2025,9 @@
       <c r="K33" s="7"/>
     </row>
     <row r="34" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="36"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C34" s="29">
         <v>43966</v>
@@ -2049,10 +2047,10 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A35" s="36"/>
+    <row r="35" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="39"/>
       <c r="B35" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C35" s="29">
         <v>43966</v>
@@ -2072,10 +2070,10 @@
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="36"/>
+    <row r="36" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A36" s="39"/>
       <c r="B36" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C36" s="29">
         <v>43966</v>
@@ -2095,12 +2093,10 @@
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37" s="35" t="s">
-        <v>101</v>
-      </c>
+    <row r="37" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="39"/>
       <c r="B37" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C37" s="29">
         <v>43966</v>
@@ -2120,10 +2116,12 @@
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="36"/>
+    <row r="38" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="38" t="s">
+        <v>99</v>
+      </c>
       <c r="B38" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C38" s="29">
         <v>43966</v>
@@ -2143,8 +2141,8 @@
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="36"/>
+    <row r="39" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="39"/>
       <c r="B39" s="7" t="s">
         <v>89</v>
       </c>
@@ -2166,10 +2164,10 @@
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="36"/>
+    <row r="40" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="39"/>
       <c r="B40" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C40" s="29">
         <v>43966</v>
@@ -2189,10 +2187,10 @@
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="36"/>
+    <row r="41" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="39"/>
       <c r="B41" s="7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C41" s="29">
         <v>43966</v>
@@ -2212,10 +2210,10 @@
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="36"/>
+    <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="39"/>
       <c r="B42" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C42" s="29">
         <v>43966</v>
@@ -2235,10 +2233,10 @@
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="36"/>
+    <row r="43" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="39"/>
       <c r="B43" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C43" s="29">
         <v>43966</v>
@@ -2258,10 +2256,10 @@
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
     </row>
-    <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="36"/>
+    <row r="44" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44" s="39"/>
       <c r="B44" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C44" s="29">
         <v>43966</v>
@@ -2281,10 +2279,10 @@
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
     </row>
-    <row r="45" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="36"/>
+    <row r="45" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="39"/>
       <c r="B45" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C45" s="29">
         <v>43966</v>
@@ -2304,10 +2302,10 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
     </row>
-    <row r="46" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="36"/>
+    <row r="46" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="39"/>
       <c r="B46" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C46" s="29">
         <v>43966</v>
@@ -2328,9 +2326,9 @@
       <c r="K46" s="7"/>
     </row>
     <row r="47" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="36"/>
+      <c r="A47" s="39"/>
       <c r="B47" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C47" s="29">
         <v>43966</v>
@@ -2351,9 +2349,9 @@
       <c r="K47" s="7"/>
     </row>
     <row r="48" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="36"/>
+      <c r="A48" s="39"/>
       <c r="B48" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C48" s="29">
         <v>43966</v>
@@ -2374,9 +2372,9 @@
       <c r="K48" s="7"/>
     </row>
     <row r="49" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="36"/>
+      <c r="A49" s="39"/>
       <c r="B49" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C49" s="29">
         <v>43966</v>
@@ -2397,9 +2395,9 @@
       <c r="K49" s="7"/>
     </row>
     <row r="50" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="36"/>
+      <c r="A50" s="39"/>
       <c r="B50" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C50" s="29">
         <v>43966</v>
@@ -2420,9 +2418,9 @@
       <c r="K50" s="7"/>
     </row>
     <row r="51" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="36"/>
+      <c r="A51" s="39"/>
       <c r="B51" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C51" s="29">
         <v>43966</v>
@@ -2442,10 +2440,10 @@
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
     </row>
-    <row r="52" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A52" s="36"/>
+    <row r="52" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="39"/>
       <c r="B52" s="7" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="C52" s="29">
         <v>43966</v>
@@ -2466,9 +2464,9 @@
       <c r="K52" s="7"/>
     </row>
     <row r="53" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A53" s="36"/>
+      <c r="A53" s="39"/>
       <c r="B53" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C53" s="29">
         <v>43966</v>
@@ -2489,9 +2487,9 @@
       <c r="K53" s="7"/>
     </row>
     <row r="54" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A54" s="36"/>
+      <c r="A54" s="39"/>
       <c r="B54" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C54" s="29">
         <v>43966</v>
@@ -2512,9 +2510,9 @@
       <c r="K54" s="7"/>
     </row>
     <row r="55" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A55" s="36"/>
+      <c r="A55" s="39"/>
       <c r="B55" s="7" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C55" s="29">
         <v>43966</v>
@@ -2535,9 +2533,9 @@
       <c r="K55" s="7"/>
     </row>
     <row r="56" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A56" s="36"/>
+      <c r="A56" s="39"/>
       <c r="B56" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C56" s="29">
         <v>43966</v>
@@ -2558,9 +2556,9 @@
       <c r="K56" s="7"/>
     </row>
     <row r="57" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A57" s="37"/>
+      <c r="A57" s="39"/>
       <c r="B57" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C57" s="29">
         <v>43966</v>
@@ -2581,11 +2579,9 @@
       <c r="K57" s="7"/>
     </row>
     <row r="58" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A58" s="35" t="s">
-        <v>125</v>
-      </c>
+      <c r="A58" s="40"/>
       <c r="B58" s="7" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="C58" s="29">
         <v>43966</v>
@@ -2605,10 +2601,12 @@
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
     </row>
-    <row r="59" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A59" s="36"/>
+    <row r="59" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A59" s="38" t="s">
+        <v>123</v>
+      </c>
       <c r="B59" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C59" s="29">
         <v>43966</v>
@@ -2628,10 +2626,10 @@
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
     </row>
-    <row r="60" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A60" s="36"/>
+    <row r="60" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="39"/>
       <c r="B60" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C60" s="29">
         <v>43966</v>
@@ -2651,10 +2649,10 @@
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
     </row>
-    <row r="61" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A61" s="36"/>
+    <row r="61" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A61" s="39"/>
       <c r="B61" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C61" s="29">
         <v>43966</v>
@@ -2674,10 +2672,10 @@
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
     </row>
-    <row r="62" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="36"/>
+    <row r="62" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A62" s="39"/>
       <c r="B62" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C62" s="29">
         <v>43966</v>
@@ -2697,10 +2695,10 @@
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
     </row>
-    <row r="63" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A63" s="36"/>
+    <row r="63" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="39"/>
       <c r="B63" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C63" s="29">
         <v>43966</v>
@@ -2721,9 +2719,9 @@
       <c r="K63" s="7"/>
     </row>
     <row r="64" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A64" s="36"/>
+      <c r="A64" s="39"/>
       <c r="B64" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C64" s="29">
         <v>43966</v>
@@ -2744,9 +2742,9 @@
       <c r="K64" s="7"/>
     </row>
     <row r="65" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A65" s="36"/>
+      <c r="A65" s="39"/>
       <c r="B65" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C65" s="29">
         <v>43966</v>
@@ -2766,10 +2764,10 @@
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
     </row>
-    <row r="66" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A66" s="36"/>
+    <row r="66" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A66" s="39"/>
       <c r="B66" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C66" s="29">
         <v>43966</v>
@@ -2790,9 +2788,9 @@
       <c r="K66" s="7"/>
     </row>
     <row r="67" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A67" s="36"/>
+      <c r="A67" s="39"/>
       <c r="B67" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C67" s="29">
         <v>43966</v>
@@ -2812,10 +2810,10 @@
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
     </row>
-    <row r="68" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="36"/>
+    <row r="68" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="39"/>
       <c r="B68" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C68" s="29">
         <v>43966</v>
@@ -2835,10 +2833,10 @@
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
     </row>
-    <row r="69" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A69" s="36"/>
+    <row r="69" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A69" s="39"/>
       <c r="B69" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C69" s="29">
         <v>43966</v>
@@ -2859,9 +2857,9 @@
       <c r="K69" s="7"/>
     </row>
     <row r="70" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A70" s="36"/>
+      <c r="A70" s="39"/>
       <c r="B70" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C70" s="29">
         <v>43966</v>
@@ -2882,9 +2880,9 @@
       <c r="K70" s="7"/>
     </row>
     <row r="71" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A71" s="36"/>
+      <c r="A71" s="39"/>
       <c r="B71" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C71" s="29">
         <v>43966</v>
@@ -2904,10 +2902,10 @@
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
     </row>
-    <row r="72" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A72" s="37"/>
+    <row r="72" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A72" s="39"/>
       <c r="B72" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C72" s="29">
         <v>43966</v>
@@ -2927,12 +2925,10 @@
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
     </row>
-    <row r="73" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A73" s="35" t="s">
-        <v>136</v>
-      </c>
+    <row r="73" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A73" s="40"/>
       <c r="B73" s="7" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C73" s="29">
         <v>43966</v>
@@ -2953,9 +2949,11 @@
       <c r="K73" s="7"/>
     </row>
     <row r="74" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A74" s="36"/>
+      <c r="A74" s="38" t="s">
+        <v>134</v>
+      </c>
       <c r="B74" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C74" s="29">
         <v>43966</v>
@@ -2976,9 +2974,9 @@
       <c r="K74" s="7"/>
     </row>
     <row r="75" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A75" s="36"/>
+      <c r="A75" s="39"/>
       <c r="B75" s="7" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C75" s="29">
         <v>43966</v>
@@ -2998,10 +2996,10 @@
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
     </row>
-    <row r="76" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A76" s="36"/>
-      <c r="B76" s="25" t="s">
-        <v>138</v>
+    <row r="76" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A76" s="39"/>
+      <c r="B76" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="C76" s="29">
         <v>43966</v>
@@ -3021,10 +3019,10 @@
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
     </row>
-    <row r="77" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A77" s="36"/>
+    <row r="77" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A77" s="39"/>
       <c r="B77" s="25" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C77" s="29">
         <v>43966</v>
@@ -3033,17 +3031,21 @@
       <c r="E77" s="29">
         <v>43966</v>
       </c>
-      <c r="F77" s="26"/>
-      <c r="G77" s="27"/>
+      <c r="F77" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G77" s="27" t="s">
+        <v>29</v>
+      </c>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
     </row>
-    <row r="78" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A78" s="36"/>
+    <row r="78" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A78" s="39"/>
       <c r="B78" s="25" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C78" s="29">
         <v>43966</v>
@@ -3059,10 +3061,10 @@
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
     </row>
-    <row r="79" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A79" s="36"/>
+    <row r="79" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A79" s="39"/>
       <c r="B79" s="25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C79" s="29">
         <v>43966</v>
@@ -3079,9 +3081,9 @@
       <c r="K79" s="7"/>
     </row>
     <row r="80" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="36"/>
-      <c r="B80" s="7" t="s">
-        <v>128</v>
+      <c r="A80" s="39"/>
+      <c r="B80" s="25" t="s">
+        <v>139</v>
       </c>
       <c r="C80" s="29">
         <v>43966</v>
@@ -3090,21 +3092,17 @@
       <c r="E80" s="29">
         <v>43966</v>
       </c>
-      <c r="F80" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="G80" s="27" t="s">
-        <v>29</v>
-      </c>
+      <c r="F80" s="26"/>
+      <c r="G80" s="27"/>
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
     </row>
     <row r="81" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A81" s="36"/>
+      <c r="A81" s="39"/>
       <c r="B81" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C81" s="29">
         <v>43966</v>
@@ -3124,10 +3122,10 @@
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
     </row>
-    <row r="82" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A82" s="36"/>
+    <row r="82" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A82" s="39"/>
       <c r="B82" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C82" s="29">
         <v>43966</v>
@@ -3147,10 +3145,10 @@
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
     </row>
-    <row r="83" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A83" s="36"/>
+    <row r="83" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A83" s="39"/>
       <c r="B83" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C83" s="29">
         <v>43966</v>
@@ -3170,10 +3168,10 @@
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
     </row>
-    <row r="84" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="36"/>
+    <row r="84" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A84" s="39"/>
       <c r="B84" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C84" s="29">
         <v>43966</v>
@@ -3193,10 +3191,10 @@
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
     </row>
-    <row r="85" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A85" s="36"/>
+    <row r="85" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A85" s="39"/>
       <c r="B85" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C85" s="29">
         <v>43966</v>
@@ -3216,10 +3214,10 @@
       <c r="J85" s="7"/>
       <c r="K85" s="7"/>
     </row>
-    <row r="86" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A86" s="36"/>
+    <row r="86" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A86" s="39"/>
       <c r="B86" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C86" s="29">
         <v>43966</v>
@@ -3239,10 +3237,10 @@
       <c r="J86" s="7"/>
       <c r="K86" s="7"/>
     </row>
-    <row r="87" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A87" s="37"/>
+    <row r="87" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A87" s="39"/>
       <c r="B87" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C87" s="29">
         <v>43966</v>
@@ -3262,29 +3260,39 @@
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
     </row>
-    <row r="88" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A88" s="31" t="s">
-        <v>149</v>
-      </c>
+    <row r="88" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A88" s="40"/>
       <c r="B88" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C88" s="28">
-        <v>43970</v>
-      </c>
-      <c r="D88" s="7"/>
-      <c r="E88" s="7"/>
-      <c r="F88" s="7"/>
-      <c r="G88" s="7"/>
+        <v>133</v>
+      </c>
+      <c r="C88" s="29">
+        <v>43966</v>
+      </c>
+      <c r="D88" s="30"/>
+      <c r="E88" s="29">
+        <v>43966</v>
+      </c>
+      <c r="F88" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G88" s="27" t="s">
+        <v>29</v>
+      </c>
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A89" s="21"/>
-      <c r="B89" s="7"/>
-      <c r="C89" s="7"/>
+    <row r="89" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A89" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C89" s="28">
+        <v>43970</v>
+      </c>
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
@@ -3451,7 +3459,7 @@
       <c r="K101" s="7"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A102" s="19"/>
+      <c r="A102" s="21"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
@@ -3464,7 +3472,7 @@
       <c r="K102" s="7"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A103" s="22"/>
+      <c r="A103" s="19"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
@@ -3503,7 +3511,7 @@
       <c r="K105" s="7"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A106" s="21"/>
+      <c r="A106" s="22"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
@@ -3516,7 +3524,7 @@
       <c r="K106" s="7"/>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A107" s="19"/>
+      <c r="A107" s="21"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
@@ -3528,23 +3536,36 @@
       <c r="J107" s="7"/>
       <c r="K107" s="7"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A109" s="5" t="s">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A108" s="19"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="7"/>
+      <c r="F108" s="7"/>
+      <c r="G108" s="7"/>
+      <c r="H108" s="7"/>
+      <c r="I108" s="7"/>
+      <c r="J108" s="7"/>
+      <c r="K108" s="7"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A110" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A110" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A111" s="10" t="s">
+      <c r="A111" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A112" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A112" s="11" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" s="11" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3552,12 +3573,12 @@
   <mergeCells count="8">
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A73:A87"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A29:A36"/>
-    <mergeCell ref="A58:A72"/>
-    <mergeCell ref="A37:A57"/>
+    <mergeCell ref="A74:A88"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A30:A37"/>
+    <mergeCell ref="A59:A73"/>
+    <mergeCell ref="A38:A58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3603,10 +3624,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="41">
+      <c r="B2" s="44">
         <v>3</v>
       </c>
       <c r="C2" s="6"/>
@@ -3619,8 +3640,8 @@
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="s">
         <v>41</v>
@@ -3631,8 +3652,8 @@
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7" t="s">
         <v>42</v>
@@ -3666,108 +3687,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="46" t="s">
+      <c r="C1" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="45" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45" t="s">
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45" t="s">
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="46" t="s">
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
-      <c r="Y2" s="46"/>
-      <c r="Z2" s="46"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="46"/>
-      <c r="Y3" s="46"/>
-      <c r="Z3" s="46"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="49"/>
+      <c r="V3" s="49"/>
+      <c r="W3" s="49"/>
+      <c r="X3" s="49"/>
+      <c r="Y3" s="49"/>
+      <c r="Z3" s="49"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="12" t="s">
         <v>51</v>
       </c>

</xml_diff>